<commit_message>
Docs Revision and Updating the Defense Matrix
Refer mo nalang sa defense matrix kulang
</commit_message>
<xml_diff>
--- a/forms/DefenseMatrix.xlsx
+++ b/forms/DefenseMatrix.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anj Lasala\Documents\GitHub\InappExp\forms\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="360" yWindow="105" windowWidth="11340" windowHeight="5520"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>Thesis Defense Matrix:</t>
   </si>
@@ -34,6 +39,42 @@
   </si>
   <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>Sir. Mike Dela Fuente</t>
+  </si>
+  <si>
+    <t>Maam Ria A. Sagum</t>
+  </si>
+  <si>
+    <t>Equation for Accuracy</t>
+  </si>
+  <si>
+    <t>Computation for Specificity</t>
+  </si>
+  <si>
+    <t>Discuss TP, FP, TN, TP</t>
+  </si>
+  <si>
+    <t>Use of Post-test and Pre-Test tanggalin na</t>
+  </si>
+  <si>
+    <t>What will be your Population</t>
+  </si>
+  <si>
+    <t>Tanggalin na number 2 sa SOP</t>
+  </si>
+  <si>
+    <t>Palitan yung number 1 sa SOP ng accuracy</t>
+  </si>
+  <si>
+    <t>Hypothesis ibase sa SOP</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Sampling Technique</t>
   </si>
 </sst>
 </file>
@@ -112,11 +153,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -126,6 +168,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -174,7 +219,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -209,7 +254,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -418,16 +463,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.85546875" customWidth="1"/>
-    <col min="2" max="2" width="28" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -440,6 +485,9 @@
       <c r="A3" t="s">
         <v>1</v>
       </c>
+      <c r="B3" s="4">
+        <v>42282</v>
+      </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -457,22 +505,90 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
+      <c r="A6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+      <c r="D6" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="7" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="8" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adjust SoP and Hypothesis
*To do: Population and other churuts
</commit_message>
<xml_diff>
--- a/forms/DefenseMatrix.xlsx
+++ b/forms/DefenseMatrix.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anj Lasala\Documents\GitHub\InappExp\forms\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\InappExp\forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="11340" windowHeight="5520"/>
+    <workbookView xWindow="360" yWindow="108" windowWidth="11340" windowHeight="5520"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>Thesis Defense Matrix:</t>
   </si>
@@ -465,23 +465,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.85546875" customWidth="1"/>
-    <col min="2" max="2" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="1" max="1" width="28.88671875" customWidth="1"/>
+    <col min="2" max="2" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -489,8 +489,8 @@
         <v>42282</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -504,7 +504,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -516,7 +516,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="3" t="s">
         <v>9</v>
@@ -526,7 +526,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3" t="s">
         <v>10</v>
@@ -536,7 +536,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3" t="s">
         <v>11</v>
@@ -546,7 +546,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
         <v>12</v>
@@ -554,7 +554,7 @@
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="3" t="s">
         <v>17</v>
@@ -562,15 +562,17 @@
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-    </row>
-    <row r="13" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>7</v>
       </c>
@@ -582,13 +584,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
+      <c r="D14" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -601,7 +605,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -613,7 +617,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated defense Matrix + Revisions of Chapter 1-3
*Please refer to defense matrix for revisions
</commit_message>
<xml_diff>
--- a/forms/DefenseMatrix.xlsx
+++ b/forms/DefenseMatrix.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\InappExp\forms\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anj Lasala\Documents\GitHub\InappExp\forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="108" windowWidth="11340" windowHeight="5520"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="11340" windowHeight="5520"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
   <si>
     <t>Thesis Defense Matrix:</t>
   </si>
@@ -75,6 +75,33 @@
   </si>
   <si>
     <t>Sampling Technique</t>
+  </si>
+  <si>
+    <t>Revisions v2.0</t>
+  </si>
+  <si>
+    <t>Use convenience sampling in sampling tech</t>
+  </si>
+  <si>
+    <t>Data gathering step by step</t>
+  </si>
+  <si>
+    <t>Related Studies on: Word Filter, characteristics of inapp, how to capture inapp, expression analysis</t>
+  </si>
+  <si>
+    <t>F-measure as accuracy</t>
+  </si>
+  <si>
+    <t>Discuss Specificity</t>
+  </si>
+  <si>
+    <t>Description of Respondents to Description of Subjects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Objective of the SOP is to model inapp.. Not to develop.. </t>
+  </si>
+  <si>
+    <t>Gantt Chart</t>
   </si>
 </sst>
 </file>
@@ -98,7 +125,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -149,16 +176,55 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -463,25 +529,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.88671875" customWidth="1"/>
-    <col min="2" max="2" width="38.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="1" max="1" width="28.85546875" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -489,8 +558,8 @@
         <v>42282</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -503,8 +572,19 @@
       <c r="D5" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5" s="7"/>
+    </row>
+    <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -515,8 +595,17 @@
       <c r="D6" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="7"/>
+    </row>
+    <row r="7" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3" t="s">
         <v>9</v>
@@ -525,8 +614,17 @@
       <c r="D7" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F7" s="2"/>
+      <c r="G7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" s="7"/>
+    </row>
+    <row r="8" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3" t="s">
         <v>10</v>
@@ -535,8 +633,15 @@
       <c r="D8" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F8" s="2"/>
+      <c r="G8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="7"/>
+    </row>
+    <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3" t="s">
         <v>11</v>
@@ -545,8 +650,15 @@
       <c r="D9" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F9" s="2"/>
+      <c r="G9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="2"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="7"/>
+    </row>
+    <row r="10" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
         <v>12</v>
@@ -555,8 +667,17 @@
       <c r="D10" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F10" s="2"/>
+      <c r="G10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J10" s="7"/>
+    </row>
+    <row r="11" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3" t="s">
         <v>17</v>
@@ -565,18 +686,36 @@
       <c r="D11" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3" t="s">
+      <c r="F11" s="2"/>
+      <c r="G11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="2"/>
+      <c r="I11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J11" s="7"/>
+    </row>
+    <row r="12" spans="1:10" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="8"/>
+      <c r="D12" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12" s="5"/>
+      <c r="I12" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="J12" s="11"/>
+    </row>
+    <row r="13" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>7</v>
       </c>
@@ -587,8 +726,17 @@
       <c r="D13" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F13" s="2"/>
+      <c r="G13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" s="2"/>
+      <c r="I13" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J13" s="7"/>
+    </row>
+    <row r="14" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2" t="s">
         <v>14</v>
@@ -597,6 +745,11 @@
       <c r="D14" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -609,7 +762,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -621,7 +774,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>